<commit_message>
failed commit fix 2
</commit_message>
<xml_diff>
--- a/Documentation/Wilson Thrust BOM v4 Grip LEDs.xlsx
+++ b/Documentation/Wilson Thrust BOM v4 Grip LEDs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\noahm\Documents\GitHub\WilsonThrust510\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44109E80-42C3-4E6B-B0A4-AF886F9C465E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CFC658E-4AEC-40E1-A032-CD259F0AAD17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18000" activeTab="4" xr2:uid="{C99EEBEB-5120-4843-8B17-4416EAFBA3F3}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="458" uniqueCount="353">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="468" uniqueCount="363">
   <si>
     <t>Part no.</t>
   </si>
@@ -295,18 +295,6 @@
   </si>
   <si>
     <t>91292A005</t>
-  </si>
-  <si>
-    <t>91290A047</t>
-  </si>
-  <si>
-    <t>91292A833</t>
-  </si>
-  <si>
-    <t>91294A135</t>
-  </si>
-  <si>
-    <t>91420A118</t>
   </si>
   <si>
     <t>93395A198</t>
@@ -427,9 +415,6 @@
     <t>91305A104</t>
   </si>
   <si>
-    <t>91290A117</t>
-  </si>
-  <si>
     <t>M6 Threaded Inserts</t>
   </si>
   <si>
@@ -443,12 +428,6 @@
   </si>
   <si>
     <t>uxcell a15112300ux0387 2mmx4mmx0.5mm Fiber Motherboard Insulating Washers Spacer Red Pack of 100</t>
-  </si>
-  <si>
-    <t>3mm RC Shim Spacer Washer Stainless Steel Pack of 50 (3x5x0.3)</t>
-  </si>
-  <si>
-    <t>M3 x 5 x .3 mm Washers (Steel)</t>
   </si>
   <si>
     <t>M2 x 4 x .5 mm Paper Washers</t>
@@ -533,12 +512,6 @@
   </si>
   <si>
     <t>uxcell Insulating Washer 500Pcs 3mm x 8mm x 0.5mm Red Vulcanized Fiber Washer, Insulation Gasket for Motherboard</t>
-  </si>
-  <si>
-    <t>Only 24 needed for hat switch board insulation.</t>
-  </si>
-  <si>
-    <t>Only 16 needed for Main Control Board and Grip Bridge Board insulation.</t>
   </si>
   <si>
     <t xml:space="preserve">Any selector knob would work so long as it will fit a 1/4 in. flatted actuator stem. </t>
@@ -4017,33 +3990,6 @@
     </r>
   </si>
   <si>
-    <t>Category: M2 x 10mm Cap Screws</t>
-  </si>
-  <si>
-    <t>Category: M2 x 16mm Cap Screws</t>
-  </si>
-  <si>
-    <t>Category: M3 x 5mm Cap Screws</t>
-  </si>
-  <si>
-    <t>Category: M3 x 6mm Tapered Screws</t>
-  </si>
-  <si>
-    <t>Category: M3 x 8mm Cap Screws</t>
-  </si>
-  <si>
-    <t>Category: M3 x 8mm Tapered Screws</t>
-  </si>
-  <si>
-    <t>Category: M3 x 18mm Tapered Screws</t>
-  </si>
-  <si>
-    <t>Category: M5 x 12mm Tapered Screws</t>
-  </si>
-  <si>
-    <t>Category: M5 x 20mm Tapered Screws</t>
-  </si>
-  <si>
     <t xml:space="preserve">Countersink Angle: 90°
 Drive Style: JIS
 Drive Size: No. 0
@@ -4052,14 +3998,6 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">Thread Fit: Class 4h
-Thread Direction: Right Hand 
-Head Type: Flat
-Flat Head Profile: Standard
-System of Measurement: Metric
-</t>
-  </si>
-  <si>
     <r>
       <t xml:space="preserve">Category: </t>
     </r>
@@ -4090,6 +4028,426 @@
 Head Height: 0.6 mm
 </t>
     </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Thread Fit: Class 4h
+Thread Direction: Right Hand 
+Head Type: Flat
+Flat Head Profile: Standard
+System of Measurement: Metric
+Lot: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>25 pcs</t>
+    </r>
+  </si>
+  <si>
+    <t>Used to mount slide potentiometer.</t>
+  </si>
+  <si>
+    <t>91263A432</t>
+  </si>
+  <si>
+    <t>Lot: 50 pcs</t>
+  </si>
+  <si>
+    <t>Lot: 100 pcs</t>
+  </si>
+  <si>
+    <t>Lot: 500 pcs</t>
+  </si>
+  <si>
+    <t>Lot: 25 pcs</t>
+  </si>
+  <si>
+    <t>M3 x 5 x .2 mm Washers (Steel)</t>
+  </si>
+  <si>
+    <t>3mm RC Shim Spacer Washer Stainless Steel Pack of 50 (3x5x0.2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Diameter: 5.5mm
+Height: 2mm
+Drive Size: 2 mm
+Thread Type: Metric 
+Thread Fit: Class 6g
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Flat Head Profile: Standard
+Head Diameter: 6 mm
+Head Diameter Tolerance: -0.3 to 0 mm
+Head Height: 1.7 mm
+Drive Style: Hex 
+Drive Size: 2 mm
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Head Height: 1.7 mm
+Countersink Angle: 90°
+Drive Style: Hex 
+Drive Size: 2.1 mm
+Thread Type: Metric 
+Thread Spacing: Coarse 
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Head Height: 2.8 mm
+Countersink Angle: 90°
+Drive Style: Hex 
+Drive Size: 3 mm
+Thread Type: Metric 
+Thread Spacing: Coarse 
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Head Height: 2.5 mm
+Countersink Angle: 90°
+Drive Style: Phillips 
+Drive Size: No. 2
+Thread Type: Metric 
+Thread Spacing: Coarse 
+</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Category: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>M5 x 20mm Tapered Screws</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Thread Size: M5 
+Thread Pitch: 0.8 mm
+Length: 20 mm
+Threading: Fully Threaded
+Head Diameter: 9.2 mm
+</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Thread Fit: Class 6h
+Thread Direction: Right Hand 
+Head Type: Flat
+Flat Head Profile: Standard
+Lot: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>100 pcs</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Thread Fit: Class 6g
+Thread Direction: Right Hand
+Head Type: Flat
+Flat Head Profile: Standard
+Lot: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>100 pcs</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Category: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>M5 x 12mm Tapered Screws</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Thread Size: M5 
+Thread Pitch: 0.8 mm
+Length: 12 mm
+Threading: Fully Threaded
+Head Diameter: 10 mm
+</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Category: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>M3 x 16mm Tapered Screws</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Thread Size: M3 
+Thread Pitch: 0.5 mm
+Length: 16 mm
+Threading: Fully Threaded
+Head Diameter: 6 mm
+</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Thread Fit: Class 4g6g
+Thread Direction: Right Hand 
+Head Type: Flat
+Flat Head Profile: Standard
+Lot: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>50 pcs</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Thread Type: Metric 
+Thread Spacing: Coarse 
+Thread Fit: Class 6g
+Thread Direction: Right Hand 
+Head Type: Flat
+Lot: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>50 pcs</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Category: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>M3 x 6mm Tapered Screws</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Thread Size: M3 
+Thread Pitch: 0.5 mm
+Length: 6 mm
+Threading: Fully Threaded
+Countersink Angle: 90°
+</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Category: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>M3 x 5mm Cap Screws</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Thread Size: M3 
+Thread Pitch: 0.5 mm
+Length: 5mm
+Threading: Fully Threaded
+Thread Spacing: Coarse
+</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Thread Direction: Right Hand 
+Head Type: Socket
+Socket Head Profile: Low
+Drive Style: Hex
+Lot: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>100 pcs</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+  </si>
+  <si>
+    <t>Used to mount the main controller board.</t>
+  </si>
+  <si>
+    <t>Used for holding most of the throttle shells together and various other things.</t>
+  </si>
+  <si>
+    <t>Used for attaching the Main Throttle Grip to the throttle arm, Hold the Grip PCB in place, and attach the Grip Front Block to the Grip Main Body.</t>
+  </si>
+  <si>
+    <t>Used to attach the Flat Braces to the bottom of the Box shell.</t>
+  </si>
+  <si>
+    <t>Only used if you plan to mount the throttle instead of using it on a table or desk.</t>
   </si>
 </sst>
 </file>
@@ -4690,19 +5048,19 @@
   <sheetData>
     <row r="1" spans="1:10" ht="30" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A1" s="44" t="s">
-        <v>223</v>
+        <v>214</v>
       </c>
       <c r="B1" s="44" t="s">
-        <v>224</v>
+        <v>215</v>
       </c>
       <c r="C1" s="44" t="s">
-        <v>187</v>
+        <v>178</v>
       </c>
       <c r="D1" s="45" t="s">
-        <v>160</v>
+        <v>151</v>
       </c>
       <c r="E1" s="45" t="s">
-        <v>176</v>
+        <v>167</v>
       </c>
       <c r="F1" s="45" t="s">
         <v>1</v>
@@ -4711,18 +5069,18 @@
         <v>2</v>
       </c>
       <c r="H1" s="45" t="s">
-        <v>203</v>
+        <v>194</v>
       </c>
       <c r="I1" s="45" t="s">
         <v>31</v>
       </c>
       <c r="J1" s="45" t="s">
-        <v>222</v>
+        <v>213</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="15" thickTop="1" x14ac:dyDescent="0.4">
       <c r="A2" s="49" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
       <c r="B2" s="50"/>
       <c r="C2" s="50"/>
@@ -4742,16 +5100,16 @@
         <v>56</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>208</v>
+        <v>199</v>
       </c>
       <c r="D3" s="31" t="s">
-        <v>339</v>
+        <v>330</v>
       </c>
       <c r="E3" s="39" t="s">
-        <v>321</v>
+        <v>312</v>
       </c>
       <c r="F3" s="31" t="s">
-        <v>145</v>
+        <v>138</v>
       </c>
       <c r="G3" s="3" t="s">
         <v>3</v>
@@ -4769,16 +5127,16 @@
         <v>12</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
       <c r="D4" s="31" t="s">
-        <v>338</v>
+        <v>329</v>
       </c>
       <c r="E4" s="39" t="s">
-        <v>322</v>
+        <v>313</v>
       </c>
       <c r="F4" s="31" t="s">
-        <v>140</v>
+        <v>133</v>
       </c>
       <c r="G4" s="3" t="s">
         <v>6</v>
@@ -4787,12 +5145,12 @@
         <v>0.04</v>
       </c>
       <c r="I4" s="41" t="s">
-        <v>209</v>
+        <v>200</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A5" s="49" t="s">
-        <v>146</v>
+        <v>139</v>
       </c>
       <c r="B5" s="50"/>
       <c r="C5" s="50"/>
@@ -4812,16 +5170,16 @@
         <v>2</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>141</v>
+        <v>134</v>
       </c>
       <c r="D6" s="31" t="s">
-        <v>336</v>
+        <v>327</v>
       </c>
       <c r="E6" s="39" t="s">
-        <v>337</v>
+        <v>328</v>
       </c>
       <c r="F6" s="31" t="s">
-        <v>210</v>
+        <v>201</v>
       </c>
       <c r="G6" s="3" t="s">
         <v>6</v>
@@ -4833,7 +5191,7 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A7" s="49" t="s">
-        <v>147</v>
+        <v>140</v>
       </c>
       <c r="B7" s="50"/>
       <c r="C7" s="50"/>
@@ -4856,10 +5214,10 @@
         <v>5</v>
       </c>
       <c r="D8" s="31" t="s">
-        <v>323</v>
+        <v>314</v>
       </c>
       <c r="E8" s="39" t="s">
-        <v>324</v>
+        <v>315</v>
       </c>
       <c r="F8" s="31" t="s">
         <v>7</v>
@@ -4874,7 +5232,7 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A9" s="49" t="s">
-        <v>148</v>
+        <v>141</v>
       </c>
       <c r="B9" s="50"/>
       <c r="C9" s="50"/>
@@ -4894,16 +5252,16 @@
         <v>1</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>211</v>
+        <v>202</v>
       </c>
       <c r="D10" s="31" t="s">
-        <v>325</v>
+        <v>316</v>
       </c>
       <c r="E10" s="39" t="s">
-        <v>212</v>
+        <v>203</v>
       </c>
       <c r="F10" s="31" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
       <c r="G10" s="3" t="s">
         <v>3</v>
@@ -4915,7 +5273,7 @@
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A11" s="49" t="s">
-        <v>149</v>
+        <v>142</v>
       </c>
       <c r="B11" s="50"/>
       <c r="C11" s="50"/>
@@ -4938,10 +5296,10 @@
         <v>11</v>
       </c>
       <c r="D12" s="31" t="s">
-        <v>326</v>
+        <v>317</v>
       </c>
       <c r="F12" s="31" t="s">
-        <v>213</v>
+        <v>204</v>
       </c>
       <c r="G12" s="3" t="s">
         <v>4</v>
@@ -4950,10 +5308,10 @@
         <v>1.65</v>
       </c>
       <c r="I12" s="41" t="s">
-        <v>220</v>
+        <v>211</v>
       </c>
       <c r="J12" s="48" t="s">
-        <v>158</v>
+        <v>149</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="233.15" x14ac:dyDescent="0.4">
@@ -4967,10 +5325,10 @@
         <v>12</v>
       </c>
       <c r="D13" s="31" t="s">
-        <v>327</v>
+        <v>318</v>
       </c>
       <c r="F13" s="31" t="s">
-        <v>217</v>
+        <v>208</v>
       </c>
       <c r="G13" s="3" t="s">
         <v>4</v>
@@ -4979,7 +5337,7 @@
         <v>4.6900000000000004</v>
       </c>
       <c r="I13" s="41" t="s">
-        <v>218</v>
+        <v>209</v>
       </c>
       <c r="J13" s="48"/>
     </row>
@@ -4991,13 +5349,13 @@
         <v>1</v>
       </c>
       <c r="C14" s="31" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="D14" s="31" t="s">
-        <v>328</v>
+        <v>319</v>
       </c>
       <c r="F14" s="31" t="s">
-        <v>214</v>
+        <v>205</v>
       </c>
       <c r="G14" s="3" t="s">
         <v>4</v>
@@ -5006,7 +5364,7 @@
         <v>2.0499999999999998</v>
       </c>
       <c r="I14" s="41" t="s">
-        <v>219</v>
+        <v>210</v>
       </c>
       <c r="J14" s="48"/>
     </row>
@@ -5021,10 +5379,10 @@
         <v>13</v>
       </c>
       <c r="D15" s="31" t="s">
-        <v>329</v>
+        <v>320</v>
       </c>
       <c r="F15" s="31" t="s">
-        <v>215</v>
+        <v>206</v>
       </c>
       <c r="G15" s="3" t="s">
         <v>4</v>
@@ -5033,7 +5391,7 @@
         <v>1.96</v>
       </c>
       <c r="I15" s="41" t="s">
-        <v>220</v>
+        <v>211</v>
       </c>
       <c r="J15" s="48"/>
     </row>
@@ -5048,10 +5406,10 @@
         <v>14</v>
       </c>
       <c r="D16" s="31" t="s">
-        <v>259</v>
+        <v>250</v>
       </c>
       <c r="F16" s="31" t="s">
-        <v>216</v>
+        <v>207</v>
       </c>
       <c r="G16" s="3" t="s">
         <v>4</v>
@@ -5060,13 +5418,13 @@
         <v>6.64</v>
       </c>
       <c r="I16" s="41" t="s">
-        <v>221</v>
+        <v>212</v>
       </c>
       <c r="J16" s="48"/>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A17" s="49" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="B17" s="50"/>
       <c r="C17" s="50"/>
@@ -5089,10 +5447,10 @@
         <v>9</v>
       </c>
       <c r="D18" s="31" t="s">
-        <v>333</v>
+        <v>324</v>
       </c>
       <c r="E18" s="39" t="s">
-        <v>334</v>
+        <v>325</v>
       </c>
       <c r="F18" s="31" t="s">
         <v>15</v>
@@ -5112,13 +5470,13 @@
         <v>1</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>159</v>
+        <v>150</v>
       </c>
       <c r="D19" s="31" t="s">
-        <v>330</v>
+        <v>321</v>
       </c>
       <c r="E19" s="39" t="s">
-        <v>335</v>
+        <v>326</v>
       </c>
       <c r="F19" s="31" t="s">
         <v>16</v>
@@ -5141,10 +5499,10 @@
         <v>10</v>
       </c>
       <c r="D20" s="31" t="s">
-        <v>331</v>
+        <v>322</v>
       </c>
       <c r="E20" s="39" t="s">
-        <v>332</v>
+        <v>323</v>
       </c>
       <c r="F20" s="31" t="s">
         <v>17</v>
@@ -5156,7 +5514,7 @@
         <v>10.97</v>
       </c>
       <c r="I20" s="41" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
     </row>
   </sheetData>
@@ -5213,28 +5571,28 @@
   <sheetData>
     <row r="1" spans="1:9" ht="15.45" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A1" s="44" t="s">
-        <v>223</v>
+        <v>214</v>
       </c>
       <c r="B1" s="44" t="s">
-        <v>224</v>
+        <v>215</v>
       </c>
       <c r="C1" s="44" t="s">
-        <v>187</v>
+        <v>178</v>
       </c>
       <c r="D1" s="45" t="s">
-        <v>160</v>
+        <v>151</v>
       </c>
       <c r="E1" s="45" t="s">
-        <v>176</v>
+        <v>167</v>
       </c>
       <c r="F1" s="45" t="s">
-        <v>229</v>
+        <v>220</v>
       </c>
       <c r="G1" s="44" t="s">
         <v>2</v>
       </c>
       <c r="H1" s="45" t="s">
-        <v>203</v>
+        <v>194</v>
       </c>
       <c r="I1" s="45" t="s">
         <v>31</v>
@@ -5251,13 +5609,13 @@
         <v>18</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>319</v>
+        <v>310</v>
       </c>
       <c r="E2" s="39" t="s">
-        <v>315</v>
+        <v>306</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>163</v>
+        <v>154</v>
       </c>
       <c r="G2" s="3" t="s">
         <v>6</v>
@@ -5266,7 +5624,7 @@
         <v>0.28399999999999997</v>
       </c>
       <c r="I2" s="41" t="s">
-        <v>207</v>
+        <v>198</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="131.15" x14ac:dyDescent="0.4">
@@ -5280,13 +5638,13 @@
         <v>19</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>318</v>
+        <v>309</v>
       </c>
       <c r="E3" s="39" t="s">
-        <v>316</v>
+        <v>307</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="G3" s="3" t="s">
         <v>6</v>
@@ -5295,7 +5653,7 @@
         <v>7.2999999999999995E-2</v>
       </c>
       <c r="I3" s="41" t="s">
-        <v>205</v>
+        <v>196</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="131.15" x14ac:dyDescent="0.4">
@@ -5309,13 +5667,13 @@
         <v>20</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>317</v>
+        <v>308</v>
       </c>
       <c r="E4" s="39" t="s">
-        <v>320</v>
+        <v>311</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>162</v>
+        <v>153</v>
       </c>
       <c r="G4" s="3" t="s">
         <v>6</v>
@@ -5324,7 +5682,7 @@
         <v>0.125</v>
       </c>
       <c r="I4" s="41" t="s">
-        <v>206</v>
+        <v>197</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.4">
@@ -5397,31 +5755,31 @@
   <sheetData>
     <row r="1" spans="1:10" ht="15.45" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A1" s="44" t="s">
-        <v>223</v>
+        <v>214</v>
       </c>
       <c r="B1" s="44" t="s">
-        <v>224</v>
+        <v>215</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>187</v>
+        <v>178</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>160</v>
+        <v>151</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>176</v>
+        <v>167</v>
       </c>
       <c r="F1" s="7" t="s">
-        <v>230</v>
+        <v>221</v>
       </c>
       <c r="G1" s="44" t="s">
-        <v>229</v>
+        <v>220</v>
       </c>
       <c r="H1" s="44" t="s">
         <v>2</v>
       </c>
       <c r="I1" s="45" t="s">
-        <v>203</v>
+        <v>194</v>
       </c>
       <c r="J1" s="45" t="s">
         <v>31</v>
@@ -5449,16 +5807,16 @@
         <v>2</v>
       </c>
       <c r="C3" s="36" t="s">
-        <v>201</v>
+        <v>192</v>
       </c>
       <c r="D3" s="36" t="s">
-        <v>258</v>
+        <v>249</v>
       </c>
       <c r="E3" s="39" t="s">
-        <v>274</v>
+        <v>265</v>
       </c>
       <c r="G3" s="36" t="s">
-        <v>202</v>
+        <v>193</v>
       </c>
       <c r="H3" s="3" t="s">
         <v>3</v>
@@ -5467,7 +5825,7 @@
         <v>13.69</v>
       </c>
       <c r="J3" s="37" t="s">
-        <v>164</v>
+        <v>155</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="145.75" x14ac:dyDescent="0.4">
@@ -5481,16 +5839,16 @@
         <v>22</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>283</v>
+        <v>274</v>
       </c>
       <c r="E4" s="39" t="s">
-        <v>285</v>
+        <v>276</v>
       </c>
       <c r="F4" s="42" t="s">
-        <v>284</v>
+        <v>275</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
       <c r="H4" s="3" t="s">
         <v>6</v>
@@ -5507,19 +5865,19 @@
         <v>1</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>280</v>
+        <v>271</v>
       </c>
       <c r="E5" s="39" t="s">
-        <v>281</v>
+        <v>272</v>
       </c>
       <c r="F5" s="42" t="s">
-        <v>282</v>
+        <v>273</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="H5" s="3" t="s">
         <v>8</v>
@@ -5554,13 +5912,13 @@
         <v>24</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>286</v>
+        <v>277</v>
       </c>
       <c r="E7" s="39" t="s">
-        <v>287</v>
+        <v>278</v>
       </c>
       <c r="F7" s="42" t="s">
-        <v>288</v>
+        <v>279</v>
       </c>
       <c r="G7" s="2" t="s">
         <v>25</v>
@@ -5584,13 +5942,13 @@
         <v>26</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>289</v>
+        <v>280</v>
       </c>
       <c r="E8" s="39" t="s">
-        <v>290</v>
+        <v>281</v>
       </c>
       <c r="F8" s="42" t="s">
-        <v>291</v>
+        <v>282</v>
       </c>
       <c r="G8" s="2" t="s">
         <v>27</v>
@@ -5625,16 +5983,16 @@
         <v>1</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>294</v>
+        <v>285</v>
       </c>
       <c r="E10" s="39" t="s">
-        <v>292</v>
+        <v>283</v>
       </c>
       <c r="F10" s="42" t="s">
-        <v>293</v>
+        <v>284</v>
       </c>
       <c r="G10" s="2" t="s">
         <v>63</v>
@@ -5649,7 +6007,7 @@
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A11" s="49" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
       <c r="B11" s="50"/>
       <c r="C11" s="50"/>
@@ -5669,16 +6027,16 @@
         <v>2</v>
       </c>
       <c r="C12" s="28" t="s">
-        <v>199</v>
+        <v>190</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>295</v>
+        <v>286</v>
       </c>
       <c r="E12" s="39" t="s">
-        <v>296</v>
+        <v>287</v>
       </c>
       <c r="F12" s="42" t="s">
-        <v>297</v>
+        <v>288</v>
       </c>
       <c r="G12" s="2" t="s">
         <v>28</v>
@@ -5699,19 +6057,19 @@
         <v>1</v>
       </c>
       <c r="C13" s="28" t="s">
-        <v>200</v>
+        <v>191</v>
       </c>
       <c r="D13" s="25" t="s">
-        <v>298</v>
+        <v>289</v>
       </c>
       <c r="E13" s="39" t="s">
-        <v>296</v>
+        <v>287</v>
       </c>
       <c r="F13" s="42" t="s">
-        <v>299</v>
+        <v>290</v>
       </c>
       <c r="G13" s="25" t="s">
-        <v>136</v>
+        <v>129</v>
       </c>
       <c r="H13" s="3" t="s">
         <v>3</v>
@@ -5720,7 +6078,7 @@
         <v>10.89</v>
       </c>
       <c r="J13" s="26" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.4">
@@ -5748,16 +6106,16 @@
         <v>30</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>300</v>
+        <v>291</v>
       </c>
       <c r="E15" s="39" t="s">
-        <v>301</v>
+        <v>292</v>
       </c>
       <c r="F15" s="42" t="s">
-        <v>302</v>
+        <v>293</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>226</v>
+        <v>217</v>
       </c>
       <c r="H15" s="3" t="s">
         <v>8</v>
@@ -5769,7 +6127,7 @@
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A16" s="49" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="B16" s="50"/>
       <c r="C16" s="50"/>
@@ -5792,13 +6150,13 @@
         <v>32</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>305</v>
+        <v>296</v>
       </c>
       <c r="E17" s="39" t="s">
-        <v>304</v>
+        <v>295</v>
       </c>
       <c r="F17" s="42" t="s">
-        <v>303</v>
+        <v>294</v>
       </c>
       <c r="G17" s="2" t="s">
         <v>33</v>
@@ -5824,16 +6182,16 @@
         <v>34</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>277</v>
+        <v>268</v>
       </c>
       <c r="E18" s="39" t="s">
-        <v>265</v>
+        <v>256</v>
       </c>
       <c r="F18" s="42" t="s">
-        <v>276</v>
+        <v>267</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="H18" s="3" t="s">
         <v>6</v>
@@ -5854,13 +6212,13 @@
         <v>35</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>306</v>
+        <v>297</v>
       </c>
       <c r="E19" s="39" t="s">
-        <v>307</v>
+        <v>298</v>
       </c>
       <c r="F19" s="42" t="s">
-        <v>308</v>
+        <v>299</v>
       </c>
       <c r="G19" s="9" t="s">
         <v>36</v>
@@ -5886,13 +6244,13 @@
         <v>39</v>
       </c>
       <c r="D20" s="23" t="s">
-        <v>278</v>
+        <v>269</v>
       </c>
       <c r="E20" s="39" t="s">
-        <v>279</v>
+        <v>270</v>
       </c>
       <c r="G20" s="23" t="s">
-        <v>204</v>
+        <v>195</v>
       </c>
       <c r="H20" s="3" t="s">
         <v>40</v>
@@ -5901,7 +6259,7 @@
         <v>5.5</v>
       </c>
       <c r="J20" s="24" t="s">
-        <v>227</v>
+        <v>218</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.4">
@@ -5929,13 +6287,13 @@
         <v>42</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>275</v>
+        <v>266</v>
       </c>
       <c r="E22" s="39" t="s">
-        <v>264</v>
+        <v>255</v>
       </c>
       <c r="F22" s="42" t="s">
-        <v>266</v>
+        <v>257</v>
       </c>
       <c r="G22" s="2" t="s">
         <v>46</v>
@@ -5975,13 +6333,13 @@
         <v>45</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>311</v>
+        <v>302</v>
       </c>
       <c r="E24" s="39" t="s">
-        <v>309</v>
+        <v>300</v>
       </c>
       <c r="F24" s="42" t="s">
-        <v>310</v>
+        <v>301</v>
       </c>
       <c r="G24" s="2" t="s">
         <v>46</v>
@@ -5993,7 +6351,7 @@
         <v>6.04</v>
       </c>
       <c r="J24" s="8" t="s">
-        <v>156</v>
+        <v>147</v>
       </c>
     </row>
     <row r="25" spans="1:10" ht="72.900000000000006" x14ac:dyDescent="0.4">
@@ -6007,13 +6365,13 @@
         <v>48</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>268</v>
+        <v>259</v>
       </c>
       <c r="E25" s="39" t="s">
-        <v>270</v>
+        <v>261</v>
       </c>
       <c r="F25" s="42" t="s">
-        <v>269</v>
+        <v>260</v>
       </c>
       <c r="G25" s="2" t="s">
         <v>47</v>
@@ -6037,13 +6395,13 @@
         <v>49</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>271</v>
+        <v>262</v>
       </c>
       <c r="E26" s="39" t="s">
-        <v>272</v>
+        <v>263</v>
       </c>
       <c r="F26" s="42" t="s">
-        <v>273</v>
+        <v>264</v>
       </c>
       <c r="G26" s="2" t="s">
         <v>50</v>
@@ -6055,12 +6413,12 @@
         <v>10.09</v>
       </c>
       <c r="J26" s="8" t="s">
-        <v>157</v>
+        <v>148</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A27" s="49" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="B27" s="50"/>
       <c r="C27" s="50"/>
@@ -6080,19 +6438,19 @@
         <v>2</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
       <c r="D28" s="25" t="s">
-        <v>312</v>
+        <v>303</v>
       </c>
       <c r="E28" s="39" t="s">
-        <v>313</v>
+        <v>304</v>
       </c>
       <c r="F28" s="42" t="s">
-        <v>267</v>
+        <v>258</v>
       </c>
       <c r="G28" s="25" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
       <c r="H28" s="3" t="s">
         <v>6</v>
@@ -6101,7 +6459,7 @@
         <v>2.4900000000000002</v>
       </c>
       <c r="J28" s="43" t="s">
-        <v>314</v>
+        <v>305</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.4">
@@ -6223,28 +6581,28 @@
   <sheetData>
     <row r="1" spans="1:9" ht="15.45" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A1" s="44" t="s">
-        <v>223</v>
+        <v>214</v>
       </c>
       <c r="B1" s="44" t="s">
-        <v>224</v>
+        <v>215</v>
       </c>
       <c r="C1" s="44" t="s">
-        <v>187</v>
+        <v>178</v>
       </c>
       <c r="D1" s="45" t="s">
-        <v>160</v>
+        <v>151</v>
       </c>
       <c r="E1" s="45" t="s">
-        <v>176</v>
+        <v>167</v>
       </c>
       <c r="F1" s="44" t="s">
-        <v>229</v>
+        <v>220</v>
       </c>
       <c r="G1" s="44" t="s">
         <v>2</v>
       </c>
       <c r="H1" s="45" t="s">
-        <v>203</v>
+        <v>194</v>
       </c>
       <c r="I1" s="45" t="s">
         <v>31</v>
@@ -6274,10 +6632,10 @@
         <v>58</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>262</v>
+        <v>253</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>166</v>
+        <v>157</v>
       </c>
       <c r="G3" s="3" t="s">
         <v>59</v>
@@ -6286,7 +6644,7 @@
         <v>0.1</v>
       </c>
       <c r="I3" s="8" t="s">
-        <v>167</v>
+        <v>158</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.4">
@@ -6307,16 +6665,16 @@
         <v>1</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>228</v>
+        <v>219</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>196</v>
+        <v>187</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>261</v>
+        <v>252</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>165</v>
+        <v>156</v>
       </c>
       <c r="G5" s="3" t="s">
         <v>3</v>
@@ -6325,12 +6683,12 @@
         <v>8.99</v>
       </c>
       <c r="I5" s="8" t="s">
-        <v>168</v>
+        <v>159</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A6" s="49" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="B6" s="50"/>
       <c r="C6" s="50"/>
@@ -6346,16 +6704,16 @@
         <v>1</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>228</v>
+        <v>219</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>197</v>
+        <v>188</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>257</v>
+        <v>248</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>174</v>
+        <v>165</v>
       </c>
       <c r="G7" s="3" t="s">
         <v>3</v>
@@ -6383,19 +6741,19 @@
         <v>1</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>228</v>
+        <v>219</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>53</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>260</v>
+        <v>251</v>
       </c>
       <c r="E9" s="39" t="s">
-        <v>175</v>
+        <v>166</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="G9" s="3" t="s">
         <v>60</v>
@@ -6404,7 +6762,7 @@
         <v>9.9700000000000006</v>
       </c>
       <c r="I9" s="8" t="s">
-        <v>169</v>
+        <v>160</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.4">
@@ -6428,10 +6786,10 @@
         <v>2</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>195</v>
+        <v>186</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>256</v>
+        <v>247</v>
       </c>
       <c r="F11" s="2" t="s">
         <v>61</v>
@@ -6443,7 +6801,7 @@
         <v>7.99</v>
       </c>
       <c r="I11" s="8" t="s">
-        <v>194</v>
+        <v>185</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.4">
@@ -6467,13 +6825,13 @@
         <v>4</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>193</v>
+        <v>184</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>252</v>
+        <v>243</v>
       </c>
       <c r="E13" s="39" t="s">
-        <v>253</v>
+        <v>244</v>
       </c>
       <c r="F13" s="2" t="s">
         <v>64</v>
@@ -6485,7 +6843,7 @@
         <v>9.99</v>
       </c>
       <c r="I13" s="8" t="s">
-        <v>170</v>
+        <v>161</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.4">
@@ -6509,25 +6867,25 @@
         <v>3</v>
       </c>
       <c r="C15" s="52" t="s">
-        <v>192</v>
+        <v>183</v>
       </c>
       <c r="D15" s="53" t="s">
-        <v>254</v>
+        <v>245</v>
       </c>
       <c r="E15" s="52" t="s">
-        <v>255</v>
+        <v>246</v>
       </c>
       <c r="F15" s="53" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="G15" s="21" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="H15" s="40">
         <v>13.49</v>
       </c>
       <c r="I15" s="54" t="s">
-        <v>171</v>
+        <v>162</v>
       </c>
     </row>
     <row r="16" spans="1:9" s="22" customFormat="1" ht="84.45" customHeight="1" x14ac:dyDescent="0.4">
@@ -6538,14 +6896,14 @@
       <c r="E16" s="52"/>
       <c r="F16" s="53"/>
       <c r="G16" s="21" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="H16" s="40"/>
       <c r="I16" s="54"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A17" s="49" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="B17" s="50"/>
       <c r="C17" s="50"/>
@@ -6564,16 +6922,16 @@
         <v>1</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>191</v>
+        <v>182</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>251</v>
+        <v>242</v>
       </c>
       <c r="E18" s="39" t="s">
-        <v>198</v>
+        <v>189</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>177</v>
+        <v>168</v>
       </c>
       <c r="G18" s="3" t="s">
         <v>3</v>
@@ -6591,16 +6949,16 @@
         <v>1</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>190</v>
+        <v>181</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>250</v>
+        <v>241</v>
       </c>
       <c r="E19" s="39" t="s">
-        <v>245</v>
+        <v>236</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>178</v>
+        <v>169</v>
       </c>
       <c r="G19" s="3" t="s">
         <v>3</v>
@@ -6612,7 +6970,7 @@
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A20" s="49" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="B20" s="50"/>
       <c r="C20" s="50"/>
@@ -6631,16 +6989,16 @@
         <v>2</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>189</v>
+        <v>180</v>
       </c>
       <c r="D21" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="E21" s="39" t="s">
         <v>237</v>
       </c>
-      <c r="E21" s="39" t="s">
-        <v>246</v>
-      </c>
       <c r="F21" s="2" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="G21" s="3" t="s">
         <v>3</v>
@@ -6658,16 +7016,16 @@
         <v>1</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>188</v>
+        <v>179</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>237</v>
+        <v>228</v>
       </c>
       <c r="E22" s="39" t="s">
-        <v>247</v>
+        <v>238</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="G22" s="3" t="s">
         <v>3</v>
@@ -6685,16 +7043,16 @@
         <v>1</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>186</v>
+        <v>177</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>238</v>
+        <v>229</v>
       </c>
       <c r="E23" s="39" t="s">
-        <v>248</v>
+        <v>239</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="G23" s="3" t="s">
         <v>3</v>
@@ -6706,7 +7064,7 @@
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A24" s="49" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="B24" s="50"/>
       <c r="C24" s="50"/>
@@ -6725,16 +7083,16 @@
         <v>1</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>184</v>
+        <v>175</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>239</v>
+        <v>230</v>
       </c>
       <c r="E25" s="39" t="s">
-        <v>249</v>
+        <v>240</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="G25" s="3" t="s">
         <v>3</v>
@@ -6743,12 +7101,12 @@
         <v>8.99</v>
       </c>
       <c r="I25" s="8" t="s">
-        <v>172</v>
+        <v>163</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A26" s="49" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="B26" s="50"/>
       <c r="C26" s="50"/>
@@ -6767,27 +7125,27 @@
         <v>1</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>179</v>
+        <v>170</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>240</v>
+        <v>231</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="G27" s="3" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="H27" s="4">
         <v>1.32</v>
       </c>
       <c r="I27" s="8" t="s">
-        <v>180</v>
+        <v>171</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A28" s="49" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="B28" s="50"/>
       <c r="C28" s="50"/>
@@ -6806,16 +7164,16 @@
         <v>2</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>183</v>
+        <v>174</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>241</v>
+        <v>232</v>
       </c>
       <c r="E29" s="39" t="s">
-        <v>236</v>
+        <v>227</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="G29" s="3" t="s">
         <v>3</v>
@@ -6827,7 +7185,7 @@
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A30" s="49" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="B30" s="50"/>
       <c r="C30" s="50"/>
@@ -6846,25 +7204,25 @@
         <v>1</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>242</v>
+        <v>233</v>
       </c>
       <c r="E31" s="39" t="s">
-        <v>235</v>
+        <v>226</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="G31" s="3" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="H31" s="4">
         <v>4.55</v>
       </c>
       <c r="I31" s="48" t="s">
-        <v>173</v>
+        <v>164</v>
       </c>
     </row>
     <row r="32" spans="1:9" ht="102" x14ac:dyDescent="0.4">
@@ -6875,19 +7233,19 @@
         <v>1</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>243</v>
+        <v>234</v>
       </c>
       <c r="E32" s="39" t="s">
-        <v>233</v>
+        <v>224</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="G32" s="3" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="H32" s="4">
         <v>5.17</v>
@@ -6896,7 +7254,7 @@
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A33" s="49" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="B33" s="50"/>
       <c r="C33" s="50"/>
@@ -6915,16 +7273,16 @@
         <v>4</v>
       </c>
       <c r="C34" s="30" t="s">
-        <v>185</v>
+        <v>176</v>
       </c>
       <c r="D34" s="30" t="s">
-        <v>244</v>
+        <v>235</v>
       </c>
       <c r="E34" s="39" t="s">
-        <v>234</v>
+        <v>225</v>
       </c>
       <c r="F34" s="30" t="s">
-        <v>182</v>
+        <v>173</v>
       </c>
       <c r="G34" s="3" t="s">
         <v>3</v>
@@ -6933,12 +7291,12 @@
         <v>8.99</v>
       </c>
       <c r="I34" s="29" t="s">
-        <v>181</v>
+        <v>172</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A35" s="49" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="B35" s="50"/>
       <c r="C35" s="50"/>
@@ -6951,19 +7309,19 @@
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A36" s="1" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="G36" s="3" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="H36" s="20" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="I36" s="8"/>
     </row>
@@ -7082,11 +7440,11 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C95DF24-9A3F-4553-BF69-26B88B2716A4}">
-  <dimension ref="A1:J59"/>
+  <dimension ref="A1:J55"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -7094,7 +7452,7 @@
     <col min="1" max="2" width="15" style="1" customWidth="1"/>
     <col min="3" max="3" width="19.15234375" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="34.921875" style="2" customWidth="1"/>
-    <col min="5" max="5" width="20.23046875" style="39" customWidth="1"/>
+    <col min="5" max="5" width="33.69140625" style="39" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="27.61328125" style="39" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="36.15234375" style="2" customWidth="1"/>
     <col min="8" max="8" width="17.69140625" style="1" bestFit="1" customWidth="1"/>
@@ -7104,31 +7462,31 @@
   <sheetData>
     <row r="1" spans="1:10" ht="15.45" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A1" s="44" t="s">
-        <v>223</v>
+        <v>214</v>
       </c>
       <c r="B1" s="44" t="s">
-        <v>224</v>
+        <v>215</v>
       </c>
       <c r="C1" s="44" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="45" t="s">
-        <v>160</v>
+        <v>151</v>
       </c>
       <c r="E1" s="45" t="s">
-        <v>176</v>
+        <v>167</v>
       </c>
       <c r="F1" s="45" t="s">
-        <v>230</v>
+        <v>221</v>
       </c>
       <c r="G1" s="45" t="s">
-        <v>229</v>
+        <v>220</v>
       </c>
       <c r="H1" s="44" t="s">
         <v>2</v>
       </c>
       <c r="I1" s="44" t="s">
-        <v>203</v>
+        <v>194</v>
       </c>
       <c r="J1" s="45" t="s">
         <v>31</v>
@@ -7159,16 +7517,16 @@
         <v>79</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>340</v>
+        <v>331</v>
       </c>
       <c r="E3" s="39" t="s">
-        <v>232</v>
+        <v>223</v>
       </c>
       <c r="F3" s="39" t="s">
-        <v>263</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>231</v>
+        <v>254</v>
+      </c>
+      <c r="G3" s="42" t="s">
+        <v>222</v>
       </c>
       <c r="H3" s="3" t="s">
         <v>71</v>
@@ -7179,22 +7537,25 @@
     </row>
     <row r="4" spans="1:10" ht="102" x14ac:dyDescent="0.4">
       <c r="A4" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B4" s="1">
         <v>2</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="D4" s="27" t="s">
-        <v>352</v>
+        <v>333</v>
       </c>
       <c r="E4" s="27" t="s">
-        <v>350</v>
+        <v>332</v>
       </c>
       <c r="F4" s="27" t="s">
-        <v>351</v>
+        <v>334</v>
+      </c>
+      <c r="G4" s="42" t="s">
+        <v>335</v>
       </c>
       <c r="H4" s="3" t="s">
         <v>71</v>
@@ -7203,446 +7564,461 @@
         <v>5.94</v>
       </c>
     </row>
-    <row r="5" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:10" s="1" customFormat="1" ht="102" x14ac:dyDescent="0.4">
       <c r="A5" s="1">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="B5" s="1">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="D5" s="1" t="s">
-        <v>341</v>
+      <c r="D5" s="42" t="s">
+        <v>356</v>
+      </c>
+      <c r="E5" s="42" t="s">
+        <v>343</v>
+      </c>
+      <c r="F5" s="42" t="s">
+        <v>357</v>
+      </c>
+      <c r="G5" s="42" t="s">
+        <v>358</v>
       </c>
       <c r="H5" s="3" t="s">
         <v>71</v>
       </c>
       <c r="I5" s="5">
-        <v>6.75</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.4">
+        <v>9.7799999999999994</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" s="1" customFormat="1" ht="102" x14ac:dyDescent="0.4">
       <c r="A6" s="1">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B6" s="1">
-        <v>4</v>
+        <v>27</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="D6" s="1" t="s">
-        <v>342</v>
+      <c r="D6" s="42" t="s">
+        <v>355</v>
+      </c>
+      <c r="E6" s="42" t="s">
+        <v>344</v>
+      </c>
+      <c r="F6" s="42" t="s">
+        <v>354</v>
+      </c>
+      <c r="G6" s="42" t="s">
+        <v>359</v>
       </c>
       <c r="H6" s="3" t="s">
         <v>71</v>
       </c>
       <c r="I6" s="5">
-        <v>13.03</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.4">
+        <v>9.16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="102" x14ac:dyDescent="0.4">
       <c r="A7" s="1">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B7" s="1">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>343</v>
+        <v>336</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>352</v>
+      </c>
+      <c r="E7" s="39" t="s">
+        <v>345</v>
+      </c>
+      <c r="F7" s="39" t="s">
+        <v>353</v>
+      </c>
+      <c r="G7" s="42" t="s">
+        <v>360</v>
       </c>
       <c r="H7" s="3" t="s">
         <v>71</v>
       </c>
       <c r="I7" s="5">
-        <v>9.7799999999999994</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.4">
+        <v>11.24</v>
+      </c>
+      <c r="J7" s="8"/>
+    </row>
+    <row r="8" spans="1:10" ht="102" x14ac:dyDescent="0.4">
       <c r="A8" s="1">
-        <v>21</v>
+        <v>1</v>
       </c>
       <c r="B8" s="1">
-        <v>21</v>
+        <v>4</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>344</v>
+        <v>83</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>351</v>
+      </c>
+      <c r="E8" s="39" t="s">
+        <v>346</v>
+      </c>
+      <c r="F8" s="39" t="s">
+        <v>350</v>
+      </c>
+      <c r="G8" s="42" t="s">
+        <v>361</v>
       </c>
       <c r="H8" s="3" t="s">
         <v>71</v>
       </c>
       <c r="I8" s="5">
-        <v>9.16</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.4">
+        <v>10.35</v>
+      </c>
+      <c r="J8" s="8"/>
+    </row>
+    <row r="9" spans="1:10" ht="102" x14ac:dyDescent="0.4">
       <c r="A9" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B9" s="1">
         <v>2</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="D9" s="25" t="s">
-        <v>345</v>
-      </c>
-      <c r="E9" s="39"/>
-      <c r="F9" s="39"/>
+        <v>82</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>348</v>
+      </c>
+      <c r="E9" s="39" t="s">
+        <v>347</v>
+      </c>
+      <c r="F9" s="39" t="s">
+        <v>349</v>
+      </c>
+      <c r="G9" s="42" t="s">
+        <v>362</v>
+      </c>
       <c r="H9" s="3" t="s">
         <v>71</v>
       </c>
       <c r="I9" s="5">
-        <v>10.85</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A10" s="1">
-        <v>5</v>
-      </c>
-      <c r="B10" s="1">
-        <v>5</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>346</v>
-      </c>
-      <c r="H10" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="I10" s="5">
-        <v>2.8</v>
-      </c>
-      <c r="J10" s="8"/>
-    </row>
-    <row r="11" spans="1:10" ht="29.15" x14ac:dyDescent="0.4">
+        <v>7.4</v>
+      </c>
+      <c r="J9" s="8"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A10" s="49" t="s">
+        <v>66</v>
+      </c>
+      <c r="B10" s="50"/>
+      <c r="C10" s="50"/>
+      <c r="D10" s="50"/>
+      <c r="E10" s="50"/>
+      <c r="F10" s="50"/>
+      <c r="G10" s="50"/>
+      <c r="H10" s="50"/>
+      <c r="I10" s="50"/>
+      <c r="J10" s="50"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A11" s="1">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="B11" s="1">
-        <v>5</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>82</v>
+        <v>14</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>74</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>347</v>
+        <v>68</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>338</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>75</v>
       </c>
       <c r="H11" s="3" t="s">
         <v>71</v>
       </c>
       <c r="I11" s="5">
-        <v>14.47</v>
+        <v>17.18</v>
       </c>
       <c r="J11" s="8"/>
     </row>
-    <row r="12" spans="1:10" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A12" s="1">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B12" s="1">
-        <v>4</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>87</v>
+        <v>38</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>73</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>348</v>
+        <v>69</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>338</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>76</v>
       </c>
       <c r="H12" s="3" t="s">
         <v>71</v>
       </c>
       <c r="I12" s="5">
-        <v>10.35</v>
+        <v>16.809999999999999</v>
       </c>
       <c r="J12" s="8"/>
     </row>
-    <row r="13" spans="1:10" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A13" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B13" s="1">
-        <v>2</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>349</v>
+        <v>4</v>
+      </c>
+      <c r="C13" s="25" t="s">
+        <v>72</v>
+      </c>
+      <c r="D13" s="25" t="s">
+        <v>70</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="G13" s="25" t="s">
+        <v>76</v>
       </c>
       <c r="H13" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="I13" s="5">
-        <v>6.17</v>
-      </c>
-      <c r="J13" s="8"/>
+      <c r="I13" s="4">
+        <v>15.64</v>
+      </c>
+      <c r="J13" s="26"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A14" s="49" t="s">
-        <v>66</v>
-      </c>
-      <c r="B14" s="50"/>
-      <c r="C14" s="50"/>
-      <c r="D14" s="50"/>
-      <c r="E14" s="50"/>
-      <c r="F14" s="50"/>
-      <c r="G14" s="50"/>
-      <c r="H14" s="50"/>
-      <c r="I14" s="50"/>
-      <c r="J14" s="50"/>
+      <c r="A14" s="1">
+        <v>1</v>
+      </c>
+      <c r="B14" s="1">
+        <v>1</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="F14" s="39" t="s">
+        <v>340</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="H14" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="I14" s="4">
+        <v>12.19</v>
+      </c>
+      <c r="J14" s="8"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A15" s="1">
-        <v>14</v>
-      </c>
-      <c r="B15" s="1">
-        <v>14</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="G15" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="H15" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="I15" s="5">
-        <v>15.04</v>
-      </c>
-      <c r="J15" s="8"/>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A16" s="1">
-        <v>28</v>
-      </c>
-      <c r="B16" s="1">
-        <v>28</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="G16" s="2" t="s">
-        <v>76</v>
-      </c>
+      <c r="A15" s="49" t="s">
+        <v>67</v>
+      </c>
+      <c r="B15" s="50"/>
+      <c r="C15" s="50"/>
+      <c r="D15" s="50"/>
+      <c r="E15" s="50"/>
+      <c r="F15" s="50"/>
+      <c r="G15" s="50"/>
+      <c r="H15" s="50"/>
+      <c r="I15" s="50"/>
+      <c r="J15" s="50"/>
+    </row>
+    <row r="16" spans="1:10" s="16" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A16" s="15">
+        <v>1</v>
+      </c>
+      <c r="B16" s="14">
+        <v>1</v>
+      </c>
+      <c r="C16" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="D16" s="17" t="s">
+        <v>77</v>
+      </c>
+      <c r="E16" s="17"/>
+      <c r="F16" s="1" t="s">
+        <v>338</v>
+      </c>
+      <c r="G16" s="14"/>
       <c r="H16" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="I16" s="5">
-        <v>14.71</v>
-      </c>
-      <c r="J16" s="8"/>
+      <c r="I16" s="18">
+        <v>6.14</v>
+      </c>
+      <c r="J16" s="14"/>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A17" s="1">
-        <v>7</v>
-      </c>
-      <c r="B17" s="1">
-        <v>7</v>
-      </c>
-      <c r="C17" s="25" t="s">
-        <v>72</v>
-      </c>
-      <c r="D17" s="25" t="s">
-        <v>70</v>
-      </c>
-      <c r="G17" s="25" t="s">
-        <v>76</v>
-      </c>
-      <c r="H17" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="I17" s="4">
-        <v>13.69</v>
-      </c>
-      <c r="J17" s="26"/>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A18" s="1">
+      <c r="A17" s="49" t="s">
+        <v>118</v>
+      </c>
+      <c r="B17" s="50"/>
+      <c r="C17" s="50"/>
+      <c r="D17" s="50"/>
+      <c r="E17" s="50"/>
+      <c r="F17" s="50"/>
+      <c r="G17" s="50"/>
+      <c r="H17" s="50"/>
+      <c r="I17" s="50"/>
+      <c r="J17" s="50"/>
+    </row>
+    <row r="18" spans="1:10" s="16" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="A18" s="15">
         <v>1</v>
       </c>
-      <c r="B18" s="1">
+      <c r="B18" s="14">
+        <v>28</v>
+      </c>
+      <c r="C18" s="14" t="s">
+        <v>119</v>
+      </c>
+      <c r="D18" s="17" t="s">
+        <v>121</v>
+      </c>
+      <c r="E18" s="17"/>
+      <c r="F18" s="1" t="s">
+        <v>338</v>
+      </c>
+      <c r="G18" s="27" t="s">
+        <v>120</v>
+      </c>
+      <c r="H18" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="I18" s="18">
+        <v>7.33</v>
+      </c>
+      <c r="J18" s="34"/>
+    </row>
+    <row r="19" spans="1:10" ht="58.3" x14ac:dyDescent="0.4">
+      <c r="A19" s="33">
         <v>1</v>
       </c>
-      <c r="C18" s="2" t="s">
+      <c r="B19" s="46">
+        <v>8</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="D19" s="32" t="s">
+        <v>145</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="G19" s="32" t="s">
+        <v>146</v>
+      </c>
+      <c r="H19" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="I19" s="4">
+        <v>6.99</v>
+      </c>
+      <c r="J19" s="35"/>
+    </row>
+    <row r="20" spans="1:10" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A20" s="1">
+        <v>1</v>
+      </c>
+      <c r="B20" s="1">
+        <v>2</v>
+      </c>
+      <c r="C20" s="28" t="s">
         <v>122</v>
       </c>
-      <c r="D18" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="G18" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="H18" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="I18" s="4">
-        <v>12.19</v>
-      </c>
-      <c r="J18" s="8"/>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A19" s="49" t="s">
-        <v>67</v>
-      </c>
-      <c r="B19" s="50"/>
-      <c r="C19" s="50"/>
-      <c r="D19" s="50"/>
-      <c r="E19" s="50"/>
-      <c r="F19" s="50"/>
-      <c r="G19" s="50"/>
-      <c r="H19" s="50"/>
-      <c r="I19" s="50"/>
-      <c r="J19" s="50"/>
-    </row>
-    <row r="20" spans="1:10" s="16" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A20" s="15">
-        <v>1</v>
-      </c>
-      <c r="B20" s="14">
-        <v>1</v>
-      </c>
-      <c r="C20" s="14" t="s">
-        <v>78</v>
-      </c>
-      <c r="D20" s="17" t="s">
-        <v>77</v>
-      </c>
-      <c r="E20" s="17"/>
-      <c r="F20" s="17"/>
-      <c r="G20" s="14"/>
+      <c r="D20" s="2" t="s">
+        <v>341</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="G20" s="25" t="s">
+        <v>342</v>
+      </c>
       <c r="H20" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="I20" s="18">
-        <v>6.14</v>
-      </c>
-      <c r="J20" s="14"/>
+        <v>3</v>
+      </c>
+      <c r="I20" s="4">
+        <v>5.99</v>
+      </c>
+      <c r="J20" s="8"/>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A21" s="49" t="s">
-        <v>123</v>
-      </c>
-      <c r="B21" s="50"/>
-      <c r="C21" s="50"/>
-      <c r="D21" s="50"/>
-      <c r="E21" s="50"/>
-      <c r="F21" s="50"/>
-      <c r="G21" s="50"/>
-      <c r="H21" s="50"/>
-      <c r="I21" s="50"/>
-      <c r="J21" s="50"/>
-    </row>
-    <row r="22" spans="1:10" s="16" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
-      <c r="A22" s="15">
-        <v>1</v>
-      </c>
-      <c r="B22" s="14">
-        <v>24</v>
-      </c>
-      <c r="C22" s="14" t="s">
-        <v>124</v>
-      </c>
-      <c r="D22" s="17" t="s">
-        <v>128</v>
-      </c>
-      <c r="E22" s="17"/>
-      <c r="F22" s="17"/>
-      <c r="G22" s="27" t="s">
-        <v>125</v>
-      </c>
-      <c r="H22" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="I22" s="18">
-        <v>3.58</v>
-      </c>
-      <c r="J22" s="34" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" ht="58.3" x14ac:dyDescent="0.4">
-      <c r="A23" s="33">
-        <v>1</v>
-      </c>
-      <c r="B23" s="46">
-        <v>16</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="D23" s="32" t="s">
-        <v>152</v>
-      </c>
-      <c r="G23" s="32" t="s">
-        <v>153</v>
-      </c>
-      <c r="H23" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="I23" s="4">
-        <v>5.49</v>
-      </c>
-      <c r="J23" s="35" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A24" s="1">
-        <v>1</v>
-      </c>
-      <c r="C24" s="28" t="s">
-        <v>129</v>
-      </c>
-      <c r="D24" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="G24" s="25" t="s">
-        <v>126</v>
-      </c>
-      <c r="H24" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="I24" s="4">
-        <v>4.99</v>
-      </c>
+      <c r="H21" s="3"/>
+      <c r="J21" s="51"/>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="H22" s="3"/>
+      <c r="J22" s="51"/>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="G23" s="9"/>
+      <c r="H23" s="3"/>
+      <c r="J23" s="8"/>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="G24" s="9"/>
+      <c r="H24" s="3"/>
       <c r="J24" s="8"/>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.4">
       <c r="H25" s="3"/>
-      <c r="J25" s="51"/>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="H26" s="3"/>
-      <c r="J26" s="51"/>
+      <c r="J25" s="8"/>
+    </row>
+    <row r="26" spans="1:10" s="13" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A26" s="11"/>
+      <c r="B26" s="12"/>
+      <c r="C26" s="12"/>
+      <c r="D26" s="12"/>
+      <c r="E26" s="12"/>
+      <c r="F26" s="12"/>
+      <c r="G26" s="12"/>
+      <c r="H26" s="12"/>
+      <c r="I26" s="19"/>
+      <c r="J26" s="12"/>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="G27" s="9"/>
       <c r="H27" s="3"/>
       <c r="J27" s="8"/>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="G28" s="9"/>
-      <c r="H28" s="3"/>
-      <c r="J28" s="8"/>
+    <row r="28" spans="1:10" s="13" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A28" s="11"/>
+      <c r="B28" s="12"/>
+      <c r="C28" s="12"/>
+      <c r="D28" s="12"/>
+      <c r="E28" s="12"/>
+      <c r="F28" s="12"/>
+      <c r="G28" s="12"/>
+      <c r="H28" s="12"/>
+      <c r="I28" s="19"/>
+      <c r="J28" s="12"/>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.4">
       <c r="H29" s="3"/>
@@ -7661,82 +8037,62 @@
       <c r="J30" s="12"/>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="C31" s="2"/>
       <c r="H31" s="3"/>
       <c r="J31" s="8"/>
     </row>
-    <row r="32" spans="1:10" s="13" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A32" s="11"/>
-      <c r="B32" s="12"/>
-      <c r="C32" s="12"/>
-      <c r="D32" s="12"/>
-      <c r="E32" s="12"/>
-      <c r="F32" s="12"/>
-      <c r="G32" s="12"/>
-      <c r="H32" s="12"/>
-      <c r="I32" s="19"/>
-      <c r="J32" s="12"/>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="H32" s="3"/>
+      <c r="J32" s="8"/>
+    </row>
+    <row r="33" spans="8:10" x14ac:dyDescent="0.4">
       <c r="H33" s="3"/>
       <c r="J33" s="8"/>
     </row>
-    <row r="34" spans="1:10" s="13" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A34" s="11"/>
-      <c r="B34" s="12"/>
-      <c r="C34" s="12"/>
-      <c r="D34" s="12"/>
-      <c r="E34" s="12"/>
-      <c r="F34" s="12"/>
-      <c r="G34" s="12"/>
-      <c r="H34" s="12"/>
-      <c r="I34" s="19"/>
-      <c r="J34" s="12"/>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="C35" s="2"/>
-      <c r="H35" s="3"/>
+    <row r="34" spans="8:10" x14ac:dyDescent="0.4">
+      <c r="H34" s="3"/>
+      <c r="J34" s="8"/>
+    </row>
+    <row r="35" spans="8:10" x14ac:dyDescent="0.4">
       <c r="J35" s="8"/>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="H36" s="3"/>
+    <row r="36" spans="8:10" x14ac:dyDescent="0.4">
       <c r="J36" s="8"/>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="H37" s="3"/>
+    <row r="37" spans="8:10" x14ac:dyDescent="0.4">
       <c r="J37" s="8"/>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="H38" s="3"/>
+    <row r="38" spans="8:10" x14ac:dyDescent="0.4">
       <c r="J38" s="8"/>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="39" spans="8:10" x14ac:dyDescent="0.4">
       <c r="J39" s="8"/>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="40" spans="8:10" x14ac:dyDescent="0.4">
       <c r="J40" s="8"/>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="41" spans="8:10" x14ac:dyDescent="0.4">
       <c r="J41" s="8"/>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="42" spans="8:10" x14ac:dyDescent="0.4">
       <c r="J42" s="8"/>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="43" spans="8:10" x14ac:dyDescent="0.4">
       <c r="J43" s="8"/>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="44" spans="8:10" x14ac:dyDescent="0.4">
       <c r="J44" s="8"/>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="45" spans="8:10" x14ac:dyDescent="0.4">
       <c r="J45" s="8"/>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="46" spans="8:10" x14ac:dyDescent="0.4">
       <c r="J46" s="8"/>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="47" spans="8:10" x14ac:dyDescent="0.4">
       <c r="J47" s="8"/>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="48" spans="8:10" x14ac:dyDescent="0.4">
       <c r="J48" s="8"/>
     </row>
     <row r="49" spans="10:10" x14ac:dyDescent="0.4">
@@ -7759,50 +8115,34 @@
     </row>
     <row r="55" spans="10:10" x14ac:dyDescent="0.4">
       <c r="J55" s="8"/>
-    </row>
-    <row r="56" spans="10:10" x14ac:dyDescent="0.4">
-      <c r="J56" s="8"/>
-    </row>
-    <row r="57" spans="10:10" x14ac:dyDescent="0.4">
-      <c r="J57" s="8"/>
-    </row>
-    <row r="58" spans="10:10" x14ac:dyDescent="0.4">
-      <c r="J58" s="8"/>
-    </row>
-    <row r="59" spans="10:10" x14ac:dyDescent="0.4">
-      <c r="J59" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="5">
     <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A14:J14"/>
-    <mergeCell ref="A19:J19"/>
-    <mergeCell ref="J25:J26"/>
-    <mergeCell ref="A21:J21"/>
+    <mergeCell ref="A10:J10"/>
+    <mergeCell ref="A15:J15"/>
+    <mergeCell ref="J21:J22"/>
+    <mergeCell ref="A17:J17"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="H16" r:id="rId1" xr:uid="{6E0E6549-E26D-4CD2-8209-F1E34F65A268}"/>
-    <hyperlink ref="H18" r:id="rId2" xr:uid="{93389E4C-349E-42A6-B0E0-BDDECED9DA47}"/>
-    <hyperlink ref="H15" r:id="rId3" xr:uid="{675D907B-B60E-4874-AC4C-02EC4F636E24}"/>
-    <hyperlink ref="H20" r:id="rId4" xr:uid="{BC97F1DD-5AEF-4594-8531-53E76F2520D3}"/>
+    <hyperlink ref="H12" r:id="rId1" xr:uid="{6E0E6549-E26D-4CD2-8209-F1E34F65A268}"/>
+    <hyperlink ref="H14" r:id="rId2" xr:uid="{93389E4C-349E-42A6-B0E0-BDDECED9DA47}"/>
+    <hyperlink ref="H11" r:id="rId3" xr:uid="{675D907B-B60E-4874-AC4C-02EC4F636E24}"/>
+    <hyperlink ref="H16" r:id="rId4" xr:uid="{BC97F1DD-5AEF-4594-8531-53E76F2520D3}"/>
     <hyperlink ref="H3" r:id="rId5" xr:uid="{22BB869E-4D9A-41C3-98D7-B1787ABFCB96}"/>
     <hyperlink ref="H4" r:id="rId6" xr:uid="{11922DEA-CA78-45EF-83AD-95FFAB1A8256}"/>
-    <hyperlink ref="H5" r:id="rId7" xr:uid="{1E89C03C-1CD4-4CA4-AF08-E3B369537504}"/>
-    <hyperlink ref="H6" r:id="rId8" xr:uid="{33BBE470-E463-44B6-821F-1CA74A31F587}"/>
-    <hyperlink ref="H11" r:id="rId9" xr:uid="{D0529A49-19CA-4F13-A97C-5EB5F9EDD18D}"/>
-    <hyperlink ref="H10" r:id="rId10" xr:uid="{BFA98BF5-DED5-44EE-8B87-6BAF0FD56375}"/>
-    <hyperlink ref="H8" r:id="rId11" xr:uid="{24E26945-6271-49C3-8924-F6EB4150CBBD}"/>
-    <hyperlink ref="H7" r:id="rId12" xr:uid="{1388AB2F-0B7C-4E41-BB14-5584D21AF8A0}"/>
-    <hyperlink ref="H12" r:id="rId13" xr:uid="{8DFB78D7-E0A1-4BB5-B5F0-60531B0FEE66}"/>
-    <hyperlink ref="H13" r:id="rId14" xr:uid="{8610DCC0-5E05-4F9A-BA6B-25878823115B}"/>
-    <hyperlink ref="H9" r:id="rId15" xr:uid="{BEAFE0A2-861E-47FF-AE1D-6DBD8E3777CE}"/>
-    <hyperlink ref="H17" r:id="rId16" xr:uid="{659178E3-F717-4B6D-892B-952AAAD9E019}"/>
-    <hyperlink ref="H22" r:id="rId17" xr:uid="{071516B5-E3D0-4FEA-900C-CA8192FE000E}"/>
-    <hyperlink ref="H24" r:id="rId18" xr:uid="{FBE50A9A-67E2-4426-A37C-74AE018B908E}"/>
-    <hyperlink ref="H23" r:id="rId19" xr:uid="{59C82901-DC57-4D45-BEC6-A79244FF2640}"/>
+    <hyperlink ref="H7" r:id="rId7" xr:uid="{D0529A49-19CA-4F13-A97C-5EB5F9EDD18D}"/>
+    <hyperlink ref="H6" r:id="rId8" xr:uid="{24E26945-6271-49C3-8924-F6EB4150CBBD}"/>
+    <hyperlink ref="H5" r:id="rId9" xr:uid="{1388AB2F-0B7C-4E41-BB14-5584D21AF8A0}"/>
+    <hyperlink ref="H8" r:id="rId10" xr:uid="{8DFB78D7-E0A1-4BB5-B5F0-60531B0FEE66}"/>
+    <hyperlink ref="H9" r:id="rId11" xr:uid="{8610DCC0-5E05-4F9A-BA6B-25878823115B}"/>
+    <hyperlink ref="H13" r:id="rId12" xr:uid="{659178E3-F717-4B6D-892B-952AAAD9E019}"/>
+    <hyperlink ref="H18" r:id="rId13" xr:uid="{071516B5-E3D0-4FEA-900C-CA8192FE000E}"/>
+    <hyperlink ref="H20" r:id="rId14" xr:uid="{FBE50A9A-67E2-4426-A37C-74AE018B908E}"/>
+    <hyperlink ref="H19" r:id="rId15" xr:uid="{59C82901-DC57-4D45-BEC6-A79244FF2640}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId20"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId16"/>
 </worksheet>
 </file>
 

</xml_diff>